<commit_message>
Writing new file according to variant
</commit_message>
<xml_diff>
--- a/src/_outputs/Inventory_newData.xlsx
+++ b/src/_outputs/Inventory_newData.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H105"/>
+  <dimension ref="A1:H209"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -530,8 +530,10 @@
           <t>LE14103 b</t>
         </is>
       </c>
-      <c r="E3" t="n">
-        <v>1</v>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
@@ -543,8 +545,10 @@
           <t>b</t>
         </is>
       </c>
-      <c r="H3" t="n">
-        <v>0</v>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>100</t>
+        </is>
       </c>
     </row>
     <row r="4">
@@ -726,8 +730,10 @@
           <t>LE14107 b</t>
         </is>
       </c>
-      <c r="E9" t="n">
-        <v>1</v>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
@@ -739,8 +745,10 @@
           <t>d</t>
         </is>
       </c>
-      <c r="H9" t="n">
-        <v>0</v>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
       </c>
     </row>
     <row r="10">
@@ -3764,10 +3772,8 @@
           <t>1 11012.0.03.095.001</t>
         </is>
       </c>
-      <c r="E96" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="E96" t="n">
+        <v>1</v>
       </c>
       <c r="F96" t="inlineStr">
         <is>
@@ -3779,10 +3785,8 @@
           <t>D</t>
         </is>
       </c>
-      <c r="H96" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
+      <c r="H96" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="97">
@@ -4078,6 +4082,3608 @@
         <v>1</v>
       </c>
       <c r="H105" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="n">
+        <v>1</v>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>Stage-I SW Skeleton Tack Welding</t>
+        </is>
+      </c>
+      <c r="C106" t="inlineStr">
+        <is>
+          <t>SIDE WALL SHEET</t>
+        </is>
+      </c>
+      <c r="D106" t="inlineStr">
+        <is>
+          <t>LE14251</t>
+        </is>
+      </c>
+      <c r="E106" t="n">
+        <v>1</v>
+      </c>
+      <c r="F106" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="G106" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="H106" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="n">
+        <v>2</v>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>Stage-I SW Skeleton Tack Welding</t>
+        </is>
+      </c>
+      <c r="C107" t="inlineStr">
+        <is>
+          <t>SIDE WALL FRAME WORK LHS</t>
+        </is>
+      </c>
+      <c r="D107" t="inlineStr">
+        <is>
+          <t>LE14103 b</t>
+        </is>
+      </c>
+      <c r="E107" t="n">
+        <v>1</v>
+      </c>
+      <c r="F107" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="G107" t="inlineStr">
+        <is>
+          <t>b</t>
+        </is>
+      </c>
+      <c r="H107" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="n">
+        <v>3</v>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>Stage-I SW Skeleton Tack Welding</t>
+        </is>
+      </c>
+      <c r="C108" t="inlineStr">
+        <is>
+          <t>LHB Side Wall LHS</t>
+        </is>
+      </c>
+      <c r="D108" t="inlineStr"/>
+      <c r="E108" t="n">
+        <v>1</v>
+      </c>
+      <c r="F108" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="G108" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="H108" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="n">
+        <v>4</v>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>Stage-II Robotic Spot Welding</t>
+        </is>
+      </c>
+      <c r="C109" t="inlineStr">
+        <is>
+          <t>LHB Side Wall LHS</t>
+        </is>
+      </c>
+      <c r="D109" t="inlineStr"/>
+      <c r="E109" t="n">
+        <v>1</v>
+      </c>
+      <c r="F109" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="G109" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="H109" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="n">
+        <v>5</v>
+      </c>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>Stage-II Robotic Spot Welding</t>
+        </is>
+      </c>
+      <c r="C110" t="inlineStr">
+        <is>
+          <t>LHB Side Wall LHS</t>
+        </is>
+      </c>
+      <c r="D110" t="inlineStr"/>
+      <c r="E110" t="n">
+        <v>1</v>
+      </c>
+      <c r="F110" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="G110" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="H110" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="n">
+        <v>6</v>
+      </c>
+      <c r="B111" t="inlineStr">
+        <is>
+          <t>Stage-III SW skeletion Robotic Mig Welding</t>
+        </is>
+      </c>
+      <c r="C111" t="inlineStr">
+        <is>
+          <t>LHB Side Wall LHS</t>
+        </is>
+      </c>
+      <c r="D111" t="inlineStr"/>
+      <c r="E111" t="n">
+        <v>1</v>
+      </c>
+      <c r="F111" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="G111" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="H111" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="n">
+        <v>7</v>
+      </c>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t>Stage-III SW skeletion Robotic Mig Welding</t>
+        </is>
+      </c>
+      <c r="C112" t="inlineStr">
+        <is>
+          <t>LHB Side Wall LHS</t>
+        </is>
+      </c>
+      <c r="D112" t="inlineStr"/>
+      <c r="E112" t="n">
+        <v>1</v>
+      </c>
+      <c r="F112" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="G112" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="H112" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="n">
+        <v>8</v>
+      </c>
+      <c r="B113" t="inlineStr">
+        <is>
+          <t>Stage-IV Roof Bearer Robotic Arc Spot welding</t>
+        </is>
+      </c>
+      <c r="C113" t="inlineStr">
+        <is>
+          <t>CARLINE</t>
+        </is>
+      </c>
+      <c r="D113" t="inlineStr">
+        <is>
+          <t>LE14107 b</t>
+        </is>
+      </c>
+      <c r="E113" t="n">
+        <v>1</v>
+      </c>
+      <c r="F113" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="G113" t="inlineStr">
+        <is>
+          <t>d</t>
+        </is>
+      </c>
+      <c r="H113" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="n">
+        <v>9</v>
+      </c>
+      <c r="B114" t="inlineStr">
+        <is>
+          <t>Stage-IV Roof Bearer Robotic Arc Spot welding</t>
+        </is>
+      </c>
+      <c r="C114" t="inlineStr">
+        <is>
+          <t>LHB Side Wall LHS</t>
+        </is>
+      </c>
+      <c r="D114" t="inlineStr"/>
+      <c r="E114" t="n">
+        <v>1</v>
+      </c>
+      <c r="F114" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="G114" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="H114" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="n">
+        <v>10</v>
+      </c>
+      <c r="B115" t="inlineStr">
+        <is>
+          <t>Stage-IV Roof Bearer Robotic Arc Spot welding</t>
+        </is>
+      </c>
+      <c r="C115" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+      <c r="D115" t="inlineStr"/>
+      <c r="E115" t="n">
+        <v>1</v>
+      </c>
+      <c r="F115" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="G115" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+      <c r="H115" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="n">
+        <v>11</v>
+      </c>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t>Stage-V SW &amp; Roof Bearer Robotic welding</t>
+        </is>
+      </c>
+      <c r="C116" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+      <c r="D116" t="inlineStr"/>
+      <c r="E116" t="n">
+        <v>1</v>
+      </c>
+      <c r="F116" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="G116" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+      <c r="H116" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="n">
+        <v>12</v>
+      </c>
+      <c r="B117" t="inlineStr">
+        <is>
+          <t>Stage-V SW &amp; Roof Bearer Robotic welding</t>
+        </is>
+      </c>
+      <c r="C117" t="inlineStr">
+        <is>
+          <t>Welding Parts Side wall LHS</t>
+        </is>
+      </c>
+      <c r="D117" t="inlineStr">
+        <is>
+          <t>LE14196 c</t>
+        </is>
+      </c>
+      <c r="E117" t="n">
+        <v>1</v>
+      </c>
+      <c r="F117" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="G117" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="H117" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="n">
+        <v>13</v>
+      </c>
+      <c r="B118" t="inlineStr">
+        <is>
+          <t>Stage-V SW &amp; Roof Bearer Robotic welding</t>
+        </is>
+      </c>
+      <c r="C118" t="inlineStr">
+        <is>
+          <t>Side wall Left complete</t>
+        </is>
+      </c>
+      <c r="D118" t="inlineStr">
+        <is>
+          <t>LE14101 e</t>
+        </is>
+      </c>
+      <c r="E118" t="n">
+        <v>1</v>
+      </c>
+      <c r="F118" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="G118" t="n">
+        <v>4</v>
+      </c>
+      <c r="H118" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="n">
+        <v>14</v>
+      </c>
+      <c r="B119" t="inlineStr">
+        <is>
+          <t>Stage-VI Backpiece Leftover welding</t>
+        </is>
+      </c>
+      <c r="C119" t="inlineStr">
+        <is>
+          <t>Welding Parts Side wall LHS</t>
+        </is>
+      </c>
+      <c r="D119" t="inlineStr">
+        <is>
+          <t>LE14196 c</t>
+        </is>
+      </c>
+      <c r="E119" t="n">
+        <v>1</v>
+      </c>
+      <c r="F119" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="G119" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="H119" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="n">
+        <v>15</v>
+      </c>
+      <c r="B120" t="inlineStr">
+        <is>
+          <t>Stage-VI Backpiece Leftover welding</t>
+        </is>
+      </c>
+      <c r="C120" t="inlineStr">
+        <is>
+          <t>Welding Parts Side wall LHS</t>
+        </is>
+      </c>
+      <c r="D120" t="inlineStr">
+        <is>
+          <t>LE14196 c</t>
+        </is>
+      </c>
+      <c r="E120" t="n">
+        <v>1</v>
+      </c>
+      <c r="F120" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="G120" t="inlineStr">
+        <is>
+          <t>f</t>
+        </is>
+      </c>
+      <c r="H120" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="n">
+        <v>16</v>
+      </c>
+      <c r="B121" t="inlineStr">
+        <is>
+          <t>Stage I Fabrication of Sub assemblies at Tacking Jigs &amp; Fixtures , Framework tacking of Endwall Complete</t>
+        </is>
+      </c>
+      <c r="C121" t="inlineStr">
+        <is>
+          <t>ARCH COMPLETE</t>
+        </is>
+      </c>
+      <c r="D121" t="inlineStr">
+        <is>
+          <t>1 10113.0.20.120.024   A</t>
+        </is>
+      </c>
+      <c r="E121" t="n">
+        <v>1</v>
+      </c>
+      <c r="F121" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="G121" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="H121" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="n">
+        <v>17</v>
+      </c>
+      <c r="B122" t="inlineStr">
+        <is>
+          <t>Stage I Fabrication of Sub assemblies at Tacking Jigs &amp; Fixtures , Framework tacking of Endwall Complete</t>
+        </is>
+      </c>
+      <c r="C122" t="inlineStr">
+        <is>
+          <t>ARCH COMPLETE</t>
+        </is>
+      </c>
+      <c r="D122" t="inlineStr">
+        <is>
+          <t>1 10113.0.20.120.025   A</t>
+        </is>
+      </c>
+      <c r="E122" t="n">
+        <v>1</v>
+      </c>
+      <c r="F122" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="G122" t="inlineStr">
+        <is>
+          <t>b</t>
+        </is>
+      </c>
+      <c r="H122" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="n">
+        <v>18</v>
+      </c>
+      <c r="B123" t="inlineStr">
+        <is>
+          <t>Stage I Fabrication of Sub assemblies at Tacking Jigs &amp; Fixtures , Framework tacking of Endwall Complete</t>
+        </is>
+      </c>
+      <c r="C123" t="inlineStr">
+        <is>
+          <t>SILL COMPLETE</t>
+        </is>
+      </c>
+      <c r="D123" t="inlineStr">
+        <is>
+          <t>1 10113.0.20.120.020   dR</t>
+        </is>
+      </c>
+      <c r="E123" t="n">
+        <v>1</v>
+      </c>
+      <c r="F123" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="G123" t="inlineStr">
+        <is>
+          <t>c</t>
+        </is>
+      </c>
+      <c r="H123" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="n">
+        <v>19</v>
+      </c>
+      <c r="B124" t="inlineStr">
+        <is>
+          <t>Stage I Fabrication of Sub assemblies at Tacking Jigs &amp; Fixtures , Framework tacking of Endwall Complete</t>
+        </is>
+      </c>
+      <c r="C124" t="inlineStr">
+        <is>
+          <t>RAM PILLAR COMPLETE</t>
+        </is>
+      </c>
+      <c r="D124" t="inlineStr">
+        <is>
+          <t>2 10113.0.20.120.011   A</t>
+        </is>
+      </c>
+      <c r="E124" t="n">
+        <v>1</v>
+      </c>
+      <c r="F124" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="G124" t="inlineStr">
+        <is>
+          <t>d</t>
+        </is>
+      </c>
+      <c r="H124" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="n">
+        <v>20</v>
+      </c>
+      <c r="B125" t="inlineStr">
+        <is>
+          <t>Stage I Fabrication of Sub assemblies at Tacking Jigs &amp; Fixtures , Framework tacking of Endwall Complete</t>
+        </is>
+      </c>
+      <c r="C125" t="inlineStr">
+        <is>
+          <t>RAM PILLAR COMPLETE</t>
+        </is>
+      </c>
+      <c r="D125" t="inlineStr">
+        <is>
+          <t>2 10113.0.20.120.012   A</t>
+        </is>
+      </c>
+      <c r="E125" t="n">
+        <v>1</v>
+      </c>
+      <c r="F125" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="G125" t="inlineStr">
+        <is>
+          <t>e</t>
+        </is>
+      </c>
+      <c r="H125" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="n">
+        <v>21</v>
+      </c>
+      <c r="B126" t="inlineStr">
+        <is>
+          <t>Stage I Fabrication of Sub assemblies at Tacking Jigs &amp; Fixtures , Framework tacking of Endwall Complete</t>
+        </is>
+      </c>
+      <c r="C126" t="inlineStr">
+        <is>
+          <t>RAM FLANGE COMPLETE</t>
+        </is>
+      </c>
+      <c r="D126" t="inlineStr">
+        <is>
+          <t>2 10113.0.20.120.013   C</t>
+        </is>
+      </c>
+      <c r="E126" t="n">
+        <v>1</v>
+      </c>
+      <c r="F126" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="G126" t="inlineStr">
+        <is>
+          <t>f</t>
+        </is>
+      </c>
+      <c r="H126" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="n">
+        <v>22</v>
+      </c>
+      <c r="B127" t="inlineStr">
+        <is>
+          <t>Stage I Fabrication of Sub assemblies at Tacking Jigs &amp; Fixtures , Framework tacking of Endwall Complete</t>
+        </is>
+      </c>
+      <c r="C127" t="inlineStr">
+        <is>
+          <t>FRAME WORK END WALL</t>
+        </is>
+      </c>
+      <c r="D127" t="inlineStr">
+        <is>
+          <t>1 10113.0.20.120.002   I</t>
+        </is>
+      </c>
+      <c r="E127" t="n">
+        <v>1</v>
+      </c>
+      <c r="F127" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="G127" t="inlineStr">
+        <is>
+          <t>g</t>
+        </is>
+      </c>
+      <c r="H127" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="n">
+        <v>23</v>
+      </c>
+      <c r="B128" t="inlineStr">
+        <is>
+          <t>Stage I Fabrication of Sub assemblies at Tacking Jigs &amp; Fixtures , Framework tacking of Endwall Complete</t>
+        </is>
+      </c>
+      <c r="C128" t="inlineStr">
+        <is>
+          <t>End wall sheets</t>
+        </is>
+      </c>
+      <c r="D128" t="inlineStr"/>
+      <c r="E128" t="n">
+        <v>1</v>
+      </c>
+      <c r="F128" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="G128" t="inlineStr">
+        <is>
+          <t>h</t>
+        </is>
+      </c>
+      <c r="H128" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="n">
+        <v>24</v>
+      </c>
+      <c r="B129" t="inlineStr">
+        <is>
+          <t>Stage I Fabrication of Sub assemblies at Tacking Jigs &amp; Fixtures , Framework tacking of Endwall Complete</t>
+        </is>
+      </c>
+      <c r="C129" t="inlineStr">
+        <is>
+          <t>Output LHB END Wall</t>
+        </is>
+      </c>
+      <c r="D129" t="inlineStr">
+        <is>
+          <t>1 10113.0.20.120.001G</t>
+        </is>
+      </c>
+      <c r="E129" t="n">
+        <v>1</v>
+      </c>
+      <c r="F129" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="G129" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="H129" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="n">
+        <v>25</v>
+      </c>
+      <c r="B130" t="inlineStr">
+        <is>
+          <t>Stage II Robotic Endwall Welding Station</t>
+        </is>
+      </c>
+      <c r="C130" t="inlineStr">
+        <is>
+          <t>Output LHB END Wall</t>
+        </is>
+      </c>
+      <c r="D130" t="inlineStr">
+        <is>
+          <t>1 10113.0.20.120.001G</t>
+        </is>
+      </c>
+      <c r="E130" t="n">
+        <v>1</v>
+      </c>
+      <c r="F130" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="G130" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="H130" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="n">
+        <v>26</v>
+      </c>
+      <c r="B131" t="inlineStr">
+        <is>
+          <t>Stage II Robotic Endwall Welding Station</t>
+        </is>
+      </c>
+      <c r="C131" t="inlineStr">
+        <is>
+          <t>Output LHB END Wall</t>
+        </is>
+      </c>
+      <c r="D131" t="inlineStr">
+        <is>
+          <t>1 10113.0.20.120.001G</t>
+        </is>
+      </c>
+      <c r="E131" t="n">
+        <v>1</v>
+      </c>
+      <c r="F131" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="G131" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="H131" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="n">
+        <v>27</v>
+      </c>
+      <c r="B132" t="inlineStr">
+        <is>
+          <t>Stage III Manual Repair stand</t>
+        </is>
+      </c>
+      <c r="C132" t="inlineStr">
+        <is>
+          <t>Output LHB END Wall</t>
+        </is>
+      </c>
+      <c r="D132" t="inlineStr">
+        <is>
+          <t>1 10113.0.20.120.001G</t>
+        </is>
+      </c>
+      <c r="E132" t="n">
+        <v>1</v>
+      </c>
+      <c r="F132" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="G132" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="H132" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="n">
+        <v>28</v>
+      </c>
+      <c r="B133" t="inlineStr">
+        <is>
+          <t>Stage III Manual Repair stand</t>
+        </is>
+      </c>
+      <c r="C133" t="inlineStr">
+        <is>
+          <t>End wall Complete</t>
+        </is>
+      </c>
+      <c r="D133" t="inlineStr">
+        <is>
+          <t>1.10113.0.20.120.001</t>
+        </is>
+      </c>
+      <c r="E133" t="n">
+        <v>1</v>
+      </c>
+      <c r="F133" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="G133" t="n">
+        <v>5</v>
+      </c>
+      <c r="H133" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="n">
+        <v>29</v>
+      </c>
+      <c r="B134" t="inlineStr">
+        <is>
+          <t>Stage I Machine- B&amp;C machine</t>
+        </is>
+      </c>
+      <c r="C134" t="inlineStr">
+        <is>
+          <t>Roof sheeting complete</t>
+        </is>
+      </c>
+      <c r="D134" t="inlineStr">
+        <is>
+          <t>RCF-RBL-Drg-39</t>
+        </is>
+      </c>
+      <c r="E134" t="n">
+        <v>1</v>
+      </c>
+      <c r="F134" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="G134" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="H134" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="n">
+        <v>30</v>
+      </c>
+      <c r="B135" t="inlineStr">
+        <is>
+          <t>Stage I Machine- B&amp;C machine</t>
+        </is>
+      </c>
+      <c r="C135" t="inlineStr">
+        <is>
+          <t>Roof sheeting complete</t>
+        </is>
+      </c>
+      <c r="D135" t="inlineStr">
+        <is>
+          <t>RCF-RBL-Drg-39</t>
+        </is>
+      </c>
+      <c r="E135" t="n">
+        <v>1</v>
+      </c>
+      <c r="F135" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="G135" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="H135" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="n">
+        <v>31</v>
+      </c>
+      <c r="B136" t="inlineStr">
+        <is>
+          <t>Stage II Manual JIG 9.2</t>
+        </is>
+      </c>
+      <c r="C136" t="inlineStr">
+        <is>
+          <t>input for final roof arch complete</t>
+        </is>
+      </c>
+      <c r="D136" t="inlineStr">
+        <is>
+          <t>LE16112 a</t>
+        </is>
+      </c>
+      <c r="E136" t="n">
+        <v>1</v>
+      </c>
+      <c r="F136" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="G136" t="inlineStr">
+        <is>
+          <t>b</t>
+        </is>
+      </c>
+      <c r="H136" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="n">
+        <v>32</v>
+      </c>
+      <c r="B137" t="inlineStr">
+        <is>
+          <t>Stage II Manual JIG 9.2</t>
+        </is>
+      </c>
+      <c r="C137" t="inlineStr">
+        <is>
+          <t>Roof sheeting complete</t>
+        </is>
+      </c>
+      <c r="D137" t="inlineStr">
+        <is>
+          <t>RCF-RBL-Drg-39</t>
+        </is>
+      </c>
+      <c r="E137" t="n">
+        <v>1</v>
+      </c>
+      <c r="F137" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="G137" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="H137" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" t="n">
+        <v>33</v>
+      </c>
+      <c r="B138" t="inlineStr">
+        <is>
+          <t>Stage II Manual JIG 9.2</t>
+        </is>
+      </c>
+      <c r="C138" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="D138" t="inlineStr"/>
+      <c r="E138" t="n">
+        <v>1</v>
+      </c>
+      <c r="F138" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="G138" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="H138" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="n">
+        <v>34</v>
+      </c>
+      <c r="B139" t="inlineStr">
+        <is>
+          <t>Stage III Roof Robotic Welding Station</t>
+        </is>
+      </c>
+      <c r="C139" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="D139" t="inlineStr"/>
+      <c r="E139" t="n">
+        <v>1</v>
+      </c>
+      <c r="F139" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="G139" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="H139" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="n">
+        <v>35</v>
+      </c>
+      <c r="B140" t="inlineStr">
+        <is>
+          <t>Stage III Roof Robotic Welding Station</t>
+        </is>
+      </c>
+      <c r="C140" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="D140" t="inlineStr"/>
+      <c r="E140" t="n">
+        <v>1</v>
+      </c>
+      <c r="F140" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="G140" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="H140" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" t="n">
+        <v>36</v>
+      </c>
+      <c r="B141" t="inlineStr">
+        <is>
+          <t>Stage IV Roof Acceptance Stand and left over Welding station(13.0)</t>
+        </is>
+      </c>
+      <c r="C141" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="D141" t="inlineStr"/>
+      <c r="E141" t="n">
+        <v>1</v>
+      </c>
+      <c r="F141" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="G141" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="H141" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" t="n">
+        <v>37</v>
+      </c>
+      <c r="B142" t="inlineStr">
+        <is>
+          <t>Stage IV Roof Acceptance Stand and left over Welding station(13.0)</t>
+        </is>
+      </c>
+      <c r="C142" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="D142" t="inlineStr"/>
+      <c r="E142" t="n">
+        <v>1</v>
+      </c>
+      <c r="F142" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="G142" t="inlineStr">
+        <is>
+          <t>d</t>
+        </is>
+      </c>
+      <c r="H142" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" t="n">
+        <v>38</v>
+      </c>
+      <c r="B143" t="inlineStr">
+        <is>
+          <t>Stage IV Roof Acceptance Stand and left over Welding station(13.0)</t>
+        </is>
+      </c>
+      <c r="C143" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+      <c r="D143" t="inlineStr"/>
+      <c r="E143" t="n">
+        <v>1</v>
+      </c>
+      <c r="F143" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="G143" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+      <c r="H143" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="n">
+        <v>39</v>
+      </c>
+      <c r="B144" t="inlineStr">
+        <is>
+          <t>Stage V Roof Acceptance Stand and left over Welding station(11.0)</t>
+        </is>
+      </c>
+      <c r="C144" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+      <c r="D144" t="inlineStr"/>
+      <c r="E144" t="n">
+        <v>1</v>
+      </c>
+      <c r="F144" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="G144" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+      <c r="H144" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" t="n">
+        <v>40</v>
+      </c>
+      <c r="B145" t="inlineStr">
+        <is>
+          <t>Stage V Roof Acceptance Stand and left over Welding station(11.0)</t>
+        </is>
+      </c>
+      <c r="C145" t="inlineStr">
+        <is>
+          <t>Roof Complete</t>
+        </is>
+      </c>
+      <c r="D145" t="inlineStr">
+        <is>
+          <t>LE16100 f</t>
+        </is>
+      </c>
+      <c r="E145" t="n">
+        <v>1</v>
+      </c>
+      <c r="F145" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="G145" t="n">
+        <v>6</v>
+      </c>
+      <c r="H145" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="n">
+        <v>41</v>
+      </c>
+      <c r="B146" t="inlineStr">
+        <is>
+          <t>Stage I Fab:Bat Box SubAssy, Pump Mt Brkt, Elec RBC channel &amp; other cross member SubAssys</t>
+        </is>
+      </c>
+      <c r="C146" t="inlineStr">
+        <is>
+          <t>Provisions for 450L water Tank</t>
+        </is>
+      </c>
+      <c r="D146" t="inlineStr">
+        <is>
+          <t>LW11102</t>
+        </is>
+      </c>
+      <c r="E146" t="n">
+        <v>1</v>
+      </c>
+      <c r="F146" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="G146" t="inlineStr">
+        <is>
+          <t>a1</t>
+        </is>
+      </c>
+      <c r="H146" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" t="n">
+        <v>42</v>
+      </c>
+      <c r="B147" t="inlineStr">
+        <is>
+          <t>Stage I Fab:Bat Box SubAssy, Pump Mt Brkt, Elec RBC channel &amp; other cross member SubAssys</t>
+        </is>
+      </c>
+      <c r="C147" t="inlineStr">
+        <is>
+          <t>Member complete</t>
+        </is>
+      </c>
+      <c r="D147" t="inlineStr">
+        <is>
+          <t>2 10113.0.03.100.010 D</t>
+        </is>
+      </c>
+      <c r="E147" t="n">
+        <v>1</v>
+      </c>
+      <c r="F147" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="G147" t="inlineStr">
+        <is>
+          <t>a2</t>
+        </is>
+      </c>
+      <c r="H147" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" t="n">
+        <v>43</v>
+      </c>
+      <c r="B148" t="inlineStr">
+        <is>
+          <t>Stage I Fab:Bat Box SubAssy, Pump Mt Brkt, Elec RBC channel &amp; other cross member SubAssys</t>
+        </is>
+      </c>
+      <c r="C148" t="inlineStr">
+        <is>
+          <t>Crossmember complete</t>
+        </is>
+      </c>
+      <c r="D148" t="inlineStr">
+        <is>
+          <t>2 10113.0.03.100.012 A</t>
+        </is>
+      </c>
+      <c r="E148" t="n">
+        <v>1</v>
+      </c>
+      <c r="F148" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="G148" t="inlineStr">
+        <is>
+          <t>a3</t>
+        </is>
+      </c>
+      <c r="H148" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" t="n">
+        <v>44</v>
+      </c>
+      <c r="B149" t="inlineStr">
+        <is>
+          <t>Stage I Fab:Bat Box SubAssy, Pump Mt Brkt, Elec RBC channel &amp; other cross member SubAssys</t>
+        </is>
+      </c>
+      <c r="C149" t="inlineStr">
+        <is>
+          <t>Bracket complete</t>
+        </is>
+      </c>
+      <c r="D149" t="inlineStr">
+        <is>
+          <t>2 10113.0.03.100.017 A</t>
+        </is>
+      </c>
+      <c r="E149" t="n">
+        <v>1</v>
+      </c>
+      <c r="F149" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="G149" t="inlineStr">
+        <is>
+          <t>a4</t>
+        </is>
+      </c>
+      <c r="H149" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" t="n">
+        <v>45</v>
+      </c>
+      <c r="B150" t="inlineStr">
+        <is>
+          <t>Stage I Fab:Bat Box SubAssy, Pump Mt Brkt, Elec RBC channel &amp; other cross member SubAssys</t>
+        </is>
+      </c>
+      <c r="C150" t="inlineStr">
+        <is>
+          <t>BRACKET COMPLETE</t>
+        </is>
+      </c>
+      <c r="D150" t="inlineStr">
+        <is>
+          <t>2 10113.0.03.100.018</t>
+        </is>
+      </c>
+      <c r="E150" t="n">
+        <v>1</v>
+      </c>
+      <c r="F150" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="G150" t="inlineStr">
+        <is>
+          <t>a5</t>
+        </is>
+      </c>
+      <c r="H150" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" t="n">
+        <v>46</v>
+      </c>
+      <c r="B151" t="inlineStr">
+        <is>
+          <t>Stage I Fab:Bat Box SubAssy, Pump Mt Brkt, Elec RBC channel &amp; other cross member SubAssys</t>
+        </is>
+      </c>
+      <c r="C151" t="inlineStr">
+        <is>
+          <t>CROSS MEMBER COMPLETE</t>
+        </is>
+      </c>
+      <c r="D151" t="inlineStr">
+        <is>
+          <t>2 10113.1.03.100.022</t>
+        </is>
+      </c>
+      <c r="E151" t="n">
+        <v>1</v>
+      </c>
+      <c r="F151" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="G151" t="inlineStr">
+        <is>
+          <t>a6</t>
+        </is>
+      </c>
+      <c r="H151" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" t="n">
+        <v>47</v>
+      </c>
+      <c r="B152" t="inlineStr">
+        <is>
+          <t>Stage I Fab:Bat Box SubAssy, Pump Mt Brkt, Elec RBC channel &amp; other cross member SubAssys</t>
+        </is>
+      </c>
+      <c r="C152" t="inlineStr">
+        <is>
+          <t>CROSS MEMBER COMPLETE</t>
+        </is>
+      </c>
+      <c r="D152" t="inlineStr">
+        <is>
+          <t>2 10113.1.03.100.023</t>
+        </is>
+      </c>
+      <c r="E152" t="n">
+        <v>1</v>
+      </c>
+      <c r="F152" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="G152" t="inlineStr">
+        <is>
+          <t>a7</t>
+        </is>
+      </c>
+      <c r="H152" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" t="n">
+        <v>48</v>
+      </c>
+      <c r="B153" t="inlineStr">
+        <is>
+          <t>Stage I Fab:Bat Box SubAssy, Pump Mt Brkt, Elec RBC channel &amp; other cross member SubAssys</t>
+        </is>
+      </c>
+      <c r="C153" t="inlineStr">
+        <is>
+          <t>CROSS MEMBER COMPLETE</t>
+        </is>
+      </c>
+      <c r="D153" t="inlineStr">
+        <is>
+          <t>2 10113.1.03.100.024</t>
+        </is>
+      </c>
+      <c r="E153" t="n">
+        <v>1</v>
+      </c>
+      <c r="F153" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="G153" t="inlineStr">
+        <is>
+          <t>a8</t>
+        </is>
+      </c>
+      <c r="H153" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" t="n">
+        <v>49</v>
+      </c>
+      <c r="B154" t="inlineStr">
+        <is>
+          <t>Stage I Fab:Bat Box SubAssy, Pump Mt Brkt, Elec RBC channel &amp; other cross member SubAssys</t>
+        </is>
+      </c>
+      <c r="C154" t="inlineStr">
+        <is>
+          <t>Crossmember complete</t>
+        </is>
+      </c>
+      <c r="D154" t="inlineStr">
+        <is>
+          <t>LE11196</t>
+        </is>
+      </c>
+      <c r="E154" t="n">
+        <v>1</v>
+      </c>
+      <c r="F154" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="G154" t="inlineStr">
+        <is>
+          <t>a9</t>
+        </is>
+      </c>
+      <c r="H154" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" t="n">
+        <v>50</v>
+      </c>
+      <c r="B155" t="inlineStr">
+        <is>
+          <t>Stage I Fab:Bat Box SubAssy, Pump Mt Brkt, Elec RBC channel &amp; other cross member SubAssys</t>
+        </is>
+      </c>
+      <c r="C155" t="inlineStr">
+        <is>
+          <t>Crossmember complete</t>
+        </is>
+      </c>
+      <c r="D155" t="inlineStr">
+        <is>
+          <t>LE11197</t>
+        </is>
+      </c>
+      <c r="E155" t="n">
+        <v>1</v>
+      </c>
+      <c r="F155" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="G155" t="inlineStr">
+        <is>
+          <t>a10</t>
+        </is>
+      </c>
+      <c r="H155" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" t="n">
+        <v>51</v>
+      </c>
+      <c r="B156" t="inlineStr">
+        <is>
+          <t>Stage I Fab:Bat Box SubAssy, Pump Mt Brkt, Elec RBC channel &amp; other cross member SubAssys</t>
+        </is>
+      </c>
+      <c r="C156" t="inlineStr">
+        <is>
+          <t>Crossmember complete</t>
+        </is>
+      </c>
+      <c r="D156" t="inlineStr">
+        <is>
+          <t>LE11198</t>
+        </is>
+      </c>
+      <c r="E156" t="n">
+        <v>1</v>
+      </c>
+      <c r="F156" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="G156" t="inlineStr">
+        <is>
+          <t>a11</t>
+        </is>
+      </c>
+      <c r="H156" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" t="n">
+        <v>52</v>
+      </c>
+      <c r="B157" t="inlineStr">
+        <is>
+          <t>Stage I Fab:Bat Box SubAssy, Pump Mt Brkt, Elec RBC channel &amp; other cross member SubAssys</t>
+        </is>
+      </c>
+      <c r="C157" t="inlineStr">
+        <is>
+          <t>Provisions for 450L water Tank</t>
+        </is>
+      </c>
+      <c r="D157" t="inlineStr">
+        <is>
+          <t>LW11102</t>
+        </is>
+      </c>
+      <c r="E157" t="n">
+        <v>1</v>
+      </c>
+      <c r="F157" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="G157" t="inlineStr">
+        <is>
+          <t>A1</t>
+        </is>
+      </c>
+      <c r="H157" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" t="n">
+        <v>53</v>
+      </c>
+      <c r="B158" t="inlineStr">
+        <is>
+          <t>Stage I Fab:Bat Box SubAssy, Pump Mt Brkt, Elec RBC channel &amp; other cross member SubAssys</t>
+        </is>
+      </c>
+      <c r="C158" t="inlineStr">
+        <is>
+          <t>Member complete</t>
+        </is>
+      </c>
+      <c r="D158" t="inlineStr">
+        <is>
+          <t>2 10113.0.03.100.010 D</t>
+        </is>
+      </c>
+      <c r="E158" t="n">
+        <v>1</v>
+      </c>
+      <c r="F158" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="G158" t="inlineStr">
+        <is>
+          <t>A2</t>
+        </is>
+      </c>
+      <c r="H158" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" t="n">
+        <v>54</v>
+      </c>
+      <c r="B159" t="inlineStr">
+        <is>
+          <t>Stage I Fab:Bat Box SubAssy, Pump Mt Brkt, Elec RBC channel &amp; other cross member SubAssys</t>
+        </is>
+      </c>
+      <c r="C159" t="inlineStr">
+        <is>
+          <t>Crossmember complete</t>
+        </is>
+      </c>
+      <c r="D159" t="inlineStr">
+        <is>
+          <t>2 10113.0.03.100.012 A</t>
+        </is>
+      </c>
+      <c r="E159" t="n">
+        <v>1</v>
+      </c>
+      <c r="F159" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="G159" t="inlineStr">
+        <is>
+          <t>A3</t>
+        </is>
+      </c>
+      <c r="H159" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" t="n">
+        <v>55</v>
+      </c>
+      <c r="B160" t="inlineStr">
+        <is>
+          <t>Stage I Fab:Bat Box SubAssy, Pump Mt Brkt, Elec RBC channel &amp; other cross member SubAssys</t>
+        </is>
+      </c>
+      <c r="C160" t="inlineStr">
+        <is>
+          <t>Bracket complete</t>
+        </is>
+      </c>
+      <c r="D160" t="inlineStr">
+        <is>
+          <t>2 10113.0.03.100.017 A</t>
+        </is>
+      </c>
+      <c r="E160" t="n">
+        <v>1</v>
+      </c>
+      <c r="F160" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="G160" t="inlineStr">
+        <is>
+          <t>A4</t>
+        </is>
+      </c>
+      <c r="H160" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" t="n">
+        <v>56</v>
+      </c>
+      <c r="B161" t="inlineStr">
+        <is>
+          <t>Stage I Fab:Bat Box SubAssy, Pump Mt Brkt, Elec RBC channel &amp; other cross member SubAssys</t>
+        </is>
+      </c>
+      <c r="C161" t="inlineStr">
+        <is>
+          <t>BRACKET COMPLETE</t>
+        </is>
+      </c>
+      <c r="D161" t="inlineStr">
+        <is>
+          <t>2 10113.0.03.100.018</t>
+        </is>
+      </c>
+      <c r="E161" t="n">
+        <v>1</v>
+      </c>
+      <c r="F161" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="G161" t="inlineStr">
+        <is>
+          <t>A5</t>
+        </is>
+      </c>
+      <c r="H161" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" t="n">
+        <v>57</v>
+      </c>
+      <c r="B162" t="inlineStr">
+        <is>
+          <t>Stage I Fab:Bat Box SubAssy, Pump Mt Brkt, Elec RBC channel &amp; other cross member SubAssys</t>
+        </is>
+      </c>
+      <c r="C162" t="inlineStr">
+        <is>
+          <t>CROSS MEMBER COMPLETE</t>
+        </is>
+      </c>
+      <c r="D162" t="inlineStr">
+        <is>
+          <t>2 10113.1.03.100.022</t>
+        </is>
+      </c>
+      <c r="E162" t="n">
+        <v>1</v>
+      </c>
+      <c r="F162" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="G162" t="inlineStr">
+        <is>
+          <t>A6</t>
+        </is>
+      </c>
+      <c r="H162" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" t="n">
+        <v>58</v>
+      </c>
+      <c r="B163" t="inlineStr">
+        <is>
+          <t>Stage I Fab:Bat Box SubAssy, Pump Mt Brkt, Elec RBC channel &amp; other cross member SubAssys</t>
+        </is>
+      </c>
+      <c r="C163" t="inlineStr">
+        <is>
+          <t>CROSS MEMBER COMPLETE</t>
+        </is>
+      </c>
+      <c r="D163" t="inlineStr">
+        <is>
+          <t>2 10113.1.03.100.023</t>
+        </is>
+      </c>
+      <c r="E163" t="n">
+        <v>1</v>
+      </c>
+      <c r="F163" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="G163" t="inlineStr">
+        <is>
+          <t>A7</t>
+        </is>
+      </c>
+      <c r="H163" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" t="n">
+        <v>59</v>
+      </c>
+      <c r="B164" t="inlineStr">
+        <is>
+          <t>Stage I Fab:Bat Box SubAssy, Pump Mt Brkt, Elec RBC channel &amp; other cross member SubAssys</t>
+        </is>
+      </c>
+      <c r="C164" t="inlineStr">
+        <is>
+          <t>CROSS MEMBER COMPLETE</t>
+        </is>
+      </c>
+      <c r="D164" t="inlineStr">
+        <is>
+          <t>2 10113.1.03.100.024</t>
+        </is>
+      </c>
+      <c r="E164" t="n">
+        <v>1</v>
+      </c>
+      <c r="F164" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="G164" t="inlineStr">
+        <is>
+          <t>A8</t>
+        </is>
+      </c>
+      <c r="H164" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" t="n">
+        <v>60</v>
+      </c>
+      <c r="B165" t="inlineStr">
+        <is>
+          <t>Stage I Fab:Bat Box SubAssy, Pump Mt Brkt, Elec RBC channel &amp; other cross member SubAssys</t>
+        </is>
+      </c>
+      <c r="C165" t="inlineStr">
+        <is>
+          <t>Crossmember complete</t>
+        </is>
+      </c>
+      <c r="D165" t="inlineStr">
+        <is>
+          <t>LE11196</t>
+        </is>
+      </c>
+      <c r="E165" t="n">
+        <v>1</v>
+      </c>
+      <c r="F165" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="G165" t="inlineStr">
+        <is>
+          <t>A9</t>
+        </is>
+      </c>
+      <c r="H165" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" t="n">
+        <v>61</v>
+      </c>
+      <c r="B166" t="inlineStr">
+        <is>
+          <t>Stage I Fab:Bat Box SubAssy, Pump Mt Brkt, Elec RBC channel &amp; other cross member SubAssys</t>
+        </is>
+      </c>
+      <c r="C166" t="inlineStr">
+        <is>
+          <t>Crossmember complete</t>
+        </is>
+      </c>
+      <c r="D166" t="inlineStr">
+        <is>
+          <t>LE11197</t>
+        </is>
+      </c>
+      <c r="E166" t="n">
+        <v>1</v>
+      </c>
+      <c r="F166" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="G166" t="inlineStr">
+        <is>
+          <t>A10</t>
+        </is>
+      </c>
+      <c r="H166" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" t="n">
+        <v>62</v>
+      </c>
+      <c r="B167" t="inlineStr">
+        <is>
+          <t>Stage I Fab:Bat Box SubAssy, Pump Mt Brkt, Elec RBC channel &amp; other cross member SubAssys</t>
+        </is>
+      </c>
+      <c r="C167" t="inlineStr">
+        <is>
+          <t>Crossmember complete</t>
+        </is>
+      </c>
+      <c r="D167" t="inlineStr">
+        <is>
+          <t>LE11198</t>
+        </is>
+      </c>
+      <c r="E167" t="n">
+        <v>1</v>
+      </c>
+      <c r="F167" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="G167" t="inlineStr">
+        <is>
+          <t>A11</t>
+        </is>
+      </c>
+      <c r="H167" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" t="n">
+        <v>63</v>
+      </c>
+      <c r="B168" t="inlineStr">
+        <is>
+          <t>Stage II Framing, fitment &amp; welding with BO front Part  of Underframe middle parts</t>
+        </is>
+      </c>
+      <c r="C168" t="inlineStr">
+        <is>
+          <t>Provisions for 450L water Tank</t>
+        </is>
+      </c>
+      <c r="D168" t="inlineStr">
+        <is>
+          <t>LW11102</t>
+        </is>
+      </c>
+      <c r="E168" t="n">
+        <v>1</v>
+      </c>
+      <c r="F168" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="G168" t="inlineStr">
+        <is>
+          <t>A1</t>
+        </is>
+      </c>
+      <c r="H168" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" t="n">
+        <v>64</v>
+      </c>
+      <c r="B169" t="inlineStr">
+        <is>
+          <t>Stage II Framing, fitment &amp; welding with BO front Part  of Underframe middle parts</t>
+        </is>
+      </c>
+      <c r="C169" t="inlineStr">
+        <is>
+          <t>Member complete</t>
+        </is>
+      </c>
+      <c r="D169" t="inlineStr">
+        <is>
+          <t>2 10113.0.03.100.010 D</t>
+        </is>
+      </c>
+      <c r="E169" t="n">
+        <v>1</v>
+      </c>
+      <c r="F169" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="G169" t="inlineStr">
+        <is>
+          <t>A2</t>
+        </is>
+      </c>
+      <c r="H169" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" t="n">
+        <v>65</v>
+      </c>
+      <c r="B170" t="inlineStr">
+        <is>
+          <t>Stage II Framing, fitment &amp; welding with BO front Part  of Underframe middle parts</t>
+        </is>
+      </c>
+      <c r="C170" t="inlineStr">
+        <is>
+          <t>Crossmember complete</t>
+        </is>
+      </c>
+      <c r="D170" t="inlineStr">
+        <is>
+          <t>2 10113.0.03.100.012 A</t>
+        </is>
+      </c>
+      <c r="E170" t="n">
+        <v>1</v>
+      </c>
+      <c r="F170" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="G170" t="inlineStr">
+        <is>
+          <t>A3</t>
+        </is>
+      </c>
+      <c r="H170" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" t="n">
+        <v>66</v>
+      </c>
+      <c r="B171" t="inlineStr">
+        <is>
+          <t>Stage II Framing, fitment &amp; welding with BO front Part  of Underframe middle parts</t>
+        </is>
+      </c>
+      <c r="C171" t="inlineStr">
+        <is>
+          <t>Bracket complete</t>
+        </is>
+      </c>
+      <c r="D171" t="inlineStr">
+        <is>
+          <t>2 10113.0.03.100.017 A</t>
+        </is>
+      </c>
+      <c r="E171" t="n">
+        <v>1</v>
+      </c>
+      <c r="F171" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="G171" t="inlineStr">
+        <is>
+          <t>A4</t>
+        </is>
+      </c>
+      <c r="H171" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" t="n">
+        <v>67</v>
+      </c>
+      <c r="B172" t="inlineStr">
+        <is>
+          <t>Stage II Framing, fitment &amp; welding with BO front Part  of Underframe middle parts</t>
+        </is>
+      </c>
+      <c r="C172" t="inlineStr">
+        <is>
+          <t>BRACKET COMPLETE</t>
+        </is>
+      </c>
+      <c r="D172" t="inlineStr">
+        <is>
+          <t>2 10113.0.03.100.018</t>
+        </is>
+      </c>
+      <c r="E172" t="n">
+        <v>1</v>
+      </c>
+      <c r="F172" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="G172" t="inlineStr">
+        <is>
+          <t>A5</t>
+        </is>
+      </c>
+      <c r="H172" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" t="n">
+        <v>68</v>
+      </c>
+      <c r="B173" t="inlineStr">
+        <is>
+          <t>Stage II Framing, fitment &amp; welding with BO front Part  of Underframe middle parts</t>
+        </is>
+      </c>
+      <c r="C173" t="inlineStr">
+        <is>
+          <t>CROSS MEMBER COMPLETE</t>
+        </is>
+      </c>
+      <c r="D173" t="inlineStr">
+        <is>
+          <t>2 10113.1.03.100.022</t>
+        </is>
+      </c>
+      <c r="E173" t="n">
+        <v>1</v>
+      </c>
+      <c r="F173" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="G173" t="inlineStr">
+        <is>
+          <t>A6</t>
+        </is>
+      </c>
+      <c r="H173" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" t="n">
+        <v>69</v>
+      </c>
+      <c r="B174" t="inlineStr">
+        <is>
+          <t>Stage II Framing, fitment &amp; welding with BO front Part  of Underframe middle parts</t>
+        </is>
+      </c>
+      <c r="C174" t="inlineStr">
+        <is>
+          <t>CROSS MEMBER COMPLETE</t>
+        </is>
+      </c>
+      <c r="D174" t="inlineStr">
+        <is>
+          <t>2 10113.1.03.100.023</t>
+        </is>
+      </c>
+      <c r="E174" t="n">
+        <v>1</v>
+      </c>
+      <c r="F174" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="G174" t="inlineStr">
+        <is>
+          <t>A7</t>
+        </is>
+      </c>
+      <c r="H174" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" t="n">
+        <v>70</v>
+      </c>
+      <c r="B175" t="inlineStr">
+        <is>
+          <t>Stage II Framing, fitment &amp; welding with BO front Part  of Underframe middle parts</t>
+        </is>
+      </c>
+      <c r="C175" t="inlineStr">
+        <is>
+          <t>CROSS MEMBER COMPLETE</t>
+        </is>
+      </c>
+      <c r="D175" t="inlineStr">
+        <is>
+          <t>2 10113.1.03.100.024</t>
+        </is>
+      </c>
+      <c r="E175" t="n">
+        <v>1</v>
+      </c>
+      <c r="F175" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="G175" t="inlineStr">
+        <is>
+          <t>A8</t>
+        </is>
+      </c>
+      <c r="H175" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" t="n">
+        <v>71</v>
+      </c>
+      <c r="B176" t="inlineStr">
+        <is>
+          <t>Stage II Framing, fitment &amp; welding with BO front Part  of Underframe middle parts</t>
+        </is>
+      </c>
+      <c r="C176" t="inlineStr">
+        <is>
+          <t>Crossmember complete</t>
+        </is>
+      </c>
+      <c r="D176" t="inlineStr">
+        <is>
+          <t>LE11196</t>
+        </is>
+      </c>
+      <c r="E176" t="n">
+        <v>1</v>
+      </c>
+      <c r="F176" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="G176" t="inlineStr">
+        <is>
+          <t>A9</t>
+        </is>
+      </c>
+      <c r="H176" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" t="n">
+        <v>72</v>
+      </c>
+      <c r="B177" t="inlineStr">
+        <is>
+          <t>Stage II Framing, fitment &amp; welding with BO front Part  of Underframe middle parts</t>
+        </is>
+      </c>
+      <c r="C177" t="inlineStr">
+        <is>
+          <t>Crossmember complete</t>
+        </is>
+      </c>
+      <c r="D177" t="inlineStr">
+        <is>
+          <t>LE11197</t>
+        </is>
+      </c>
+      <c r="E177" t="n">
+        <v>1</v>
+      </c>
+      <c r="F177" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="G177" t="inlineStr">
+        <is>
+          <t>A10</t>
+        </is>
+      </c>
+      <c r="H177" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" t="n">
+        <v>73</v>
+      </c>
+      <c r="B178" t="inlineStr">
+        <is>
+          <t>Stage II Framing, fitment &amp; welding with BO front Part  of Underframe middle parts</t>
+        </is>
+      </c>
+      <c r="C178" t="inlineStr">
+        <is>
+          <t>Crossmember complete</t>
+        </is>
+      </c>
+      <c r="D178" t="inlineStr">
+        <is>
+          <t>LE11198</t>
+        </is>
+      </c>
+      <c r="E178" t="n">
+        <v>1</v>
+      </c>
+      <c r="F178" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="G178" t="inlineStr">
+        <is>
+          <t>A11</t>
+        </is>
+      </c>
+      <c r="H178" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" t="n">
+        <v>74</v>
+      </c>
+      <c r="B179" t="inlineStr">
+        <is>
+          <t>Stage II Framing, fitment &amp; welding with BO front Part  of Underframe middle parts</t>
+        </is>
+      </c>
+      <c r="C179" t="inlineStr">
+        <is>
+          <t>Underframe frame work</t>
+        </is>
+      </c>
+      <c r="D179" t="inlineStr">
+        <is>
+          <t>LE11269 c</t>
+        </is>
+      </c>
+      <c r="E179" t="n">
+        <v>1</v>
+      </c>
+      <c r="F179" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="G179" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="H179" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" t="n">
+        <v>75</v>
+      </c>
+      <c r="B180" t="inlineStr">
+        <is>
+          <t>Stage III Robotic Welding upside of Underframe</t>
+        </is>
+      </c>
+      <c r="C180" t="inlineStr">
+        <is>
+          <t>Underframe frame work</t>
+        </is>
+      </c>
+      <c r="D180" t="inlineStr">
+        <is>
+          <t>LE11269 c</t>
+        </is>
+      </c>
+      <c r="E180" t="n">
+        <v>1</v>
+      </c>
+      <c r="F180" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="G180" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="H180" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" t="n">
+        <v>76</v>
+      </c>
+      <c r="B181" t="inlineStr">
+        <is>
+          <t>Stage III Robotic Welding upside of Underframe</t>
+        </is>
+      </c>
+      <c r="C181" t="inlineStr">
+        <is>
+          <t>Underframe frame work</t>
+        </is>
+      </c>
+      <c r="D181" t="inlineStr">
+        <is>
+          <t>LE11269 c</t>
+        </is>
+      </c>
+      <c r="E181" t="n">
+        <v>1</v>
+      </c>
+      <c r="F181" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="G181" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="H181" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="182">
+      <c r="A182" t="n">
+        <v>77</v>
+      </c>
+      <c r="B182" t="inlineStr">
+        <is>
+          <t>Stage IV  Robotic Welding downside of Underframe</t>
+        </is>
+      </c>
+      <c r="C182" t="inlineStr">
+        <is>
+          <t>Underframe frame work</t>
+        </is>
+      </c>
+      <c r="D182" t="inlineStr">
+        <is>
+          <t>LE11269 c</t>
+        </is>
+      </c>
+      <c r="E182" t="n">
+        <v>1</v>
+      </c>
+      <c r="F182" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="G182" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="H182" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183" t="n">
+        <v>78</v>
+      </c>
+      <c r="B183" t="inlineStr">
+        <is>
+          <t>Stage IV  Robotic Welding downside of Underframe</t>
+        </is>
+      </c>
+      <c r="C183" t="inlineStr">
+        <is>
+          <t>Underframe frame work</t>
+        </is>
+      </c>
+      <c r="D183" t="inlineStr">
+        <is>
+          <t>LE11269 c</t>
+        </is>
+      </c>
+      <c r="E183" t="n">
+        <v>1</v>
+      </c>
+      <c r="F183" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="G183" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="H183" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="184">
+      <c r="A184" t="n">
+        <v>79</v>
+      </c>
+      <c r="B184" t="inlineStr">
+        <is>
+          <t>Stage V Repair &amp; leftover work by manual welding Top Side</t>
+        </is>
+      </c>
+      <c r="C184" t="inlineStr">
+        <is>
+          <t>Underframe frame work</t>
+        </is>
+      </c>
+      <c r="D184" t="inlineStr">
+        <is>
+          <t>LE11269 c</t>
+        </is>
+      </c>
+      <c r="E184" t="n">
+        <v>1</v>
+      </c>
+      <c r="F184" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="G184" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="H184" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185" t="n">
+        <v>80</v>
+      </c>
+      <c r="B185" t="inlineStr">
+        <is>
+          <t>Stage V Repair &amp; leftover work by manual welding Top Side</t>
+        </is>
+      </c>
+      <c r="C185" t="inlineStr">
+        <is>
+          <t>Underframe frame work</t>
+        </is>
+      </c>
+      <c r="D185" t="inlineStr">
+        <is>
+          <t>LE11269 c</t>
+        </is>
+      </c>
+      <c r="E185" t="n">
+        <v>1</v>
+      </c>
+      <c r="F185" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="G185" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="H185" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="186">
+      <c r="A186" t="n">
+        <v>81</v>
+      </c>
+      <c r="B186" t="inlineStr">
+        <is>
+          <t>Stage VI Corrugated Sheets Tack welded  to Underframe frame work</t>
+        </is>
+      </c>
+      <c r="C186" t="inlineStr">
+        <is>
+          <t>Trough Sheets</t>
+        </is>
+      </c>
+      <c r="D186" t="inlineStr"/>
+      <c r="E186" t="n">
+        <v>1</v>
+      </c>
+      <c r="F186" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="G186" t="inlineStr">
+        <is>
+          <t>b</t>
+        </is>
+      </c>
+      <c r="H186" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="187">
+      <c r="A187" t="n">
+        <v>82</v>
+      </c>
+      <c r="B187" t="inlineStr">
+        <is>
+          <t>Stage VI Corrugated Sheets Tack welded  to Underframe frame work</t>
+        </is>
+      </c>
+      <c r="C187" t="inlineStr">
+        <is>
+          <t>Trough Sheets</t>
+        </is>
+      </c>
+      <c r="D187" t="inlineStr"/>
+      <c r="E187" t="n">
+        <v>1</v>
+      </c>
+      <c r="F187" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="G187" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="H187" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="188">
+      <c r="A188" t="n">
+        <v>83</v>
+      </c>
+      <c r="B188" t="inlineStr">
+        <is>
+          <t>Stage VII Robotic Corrugated sheet stitch welding done</t>
+        </is>
+      </c>
+      <c r="C188" t="inlineStr">
+        <is>
+          <t>Trough Sheets</t>
+        </is>
+      </c>
+      <c r="D188" t="inlineStr"/>
+      <c r="E188" t="n">
+        <v>1</v>
+      </c>
+      <c r="F188" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="G188" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="H188" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="189">
+      <c r="A189" t="n">
+        <v>84</v>
+      </c>
+      <c r="B189" t="inlineStr">
+        <is>
+          <t>Stage VII Robotic Corrugated sheet stitch welding done</t>
+        </is>
+      </c>
+      <c r="C189" t="inlineStr">
+        <is>
+          <t>Underframe frame work</t>
+        </is>
+      </c>
+      <c r="D189" t="inlineStr">
+        <is>
+          <t>LE11269 c</t>
+        </is>
+      </c>
+      <c r="E189" t="n">
+        <v>1</v>
+      </c>
+      <c r="F189" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="G189" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="H189" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="190">
+      <c r="A190" t="n">
+        <v>85</v>
+      </c>
+      <c r="B190" t="inlineStr">
+        <is>
+          <t>Stage VII Robotic Corrugated sheet stitch welding done</t>
+        </is>
+      </c>
+      <c r="C190" t="inlineStr">
+        <is>
+          <t>Underframe frame work with corrugated sheet</t>
+        </is>
+      </c>
+      <c r="D190" t="inlineStr"/>
+      <c r="E190" t="n">
+        <v>1</v>
+      </c>
+      <c r="F190" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="G190" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="H190" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="191">
+      <c r="A191" t="n">
+        <v>86</v>
+      </c>
+      <c r="B191" t="inlineStr">
+        <is>
+          <t>Stage VIII Robotic Corrugated sheet seam welding done</t>
+        </is>
+      </c>
+      <c r="C191" t="inlineStr">
+        <is>
+          <t>Underframe frame work with corrugated sheet</t>
+        </is>
+      </c>
+      <c r="D191" t="inlineStr"/>
+      <c r="E191" t="n">
+        <v>1</v>
+      </c>
+      <c r="F191" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="G191" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="H191" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="192">
+      <c r="A192" t="n">
+        <v>87</v>
+      </c>
+      <c r="B192" t="inlineStr">
+        <is>
+          <t>Stage VIII Robotic Corrugated sheet seam welding done</t>
+        </is>
+      </c>
+      <c r="C192" t="inlineStr">
+        <is>
+          <t>Underframe frame work with corrugated sheet</t>
+        </is>
+      </c>
+      <c r="D192" t="inlineStr"/>
+      <c r="E192" t="n">
+        <v>1</v>
+      </c>
+      <c r="F192" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="G192" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="H192" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="193">
+      <c r="A193" t="n">
+        <v>88</v>
+      </c>
+      <c r="B193" t="inlineStr">
+        <is>
+          <t>Stage IX Attending of leftover work and rectification of weld defects</t>
+        </is>
+      </c>
+      <c r="C193" t="inlineStr">
+        <is>
+          <t>Underframe frame work with corrugated sheet</t>
+        </is>
+      </c>
+      <c r="D193" t="inlineStr"/>
+      <c r="E193" t="n">
+        <v>1</v>
+      </c>
+      <c r="F193" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="G193" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="H193" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="194">
+      <c r="A194" t="n">
+        <v>89</v>
+      </c>
+      <c r="B194" t="inlineStr">
+        <is>
+          <t>Stage IX Attending of leftover work and rectification of weld defects</t>
+        </is>
+      </c>
+      <c r="C194" t="inlineStr">
+        <is>
+          <t>Underframe frame work with corrugated sheet</t>
+        </is>
+      </c>
+      <c r="D194" t="inlineStr"/>
+      <c r="E194" t="n">
+        <v>1</v>
+      </c>
+      <c r="F194" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="G194" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="H194" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="195">
+      <c r="A195" t="n">
+        <v>90</v>
+      </c>
+      <c r="B195" t="inlineStr">
+        <is>
+          <t>Stage X  Manual Welding of Backpieces at Bottom side of underframe</t>
+        </is>
+      </c>
+      <c r="C195" t="inlineStr">
+        <is>
+          <t>Underframe Welding Parts</t>
+        </is>
+      </c>
+      <c r="D195" t="inlineStr">
+        <is>
+          <t>1 11012.0.03.095.001</t>
+        </is>
+      </c>
+      <c r="E195" t="n">
+        <v>1</v>
+      </c>
+      <c r="F195" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="G195" t="inlineStr">
+        <is>
+          <t>d</t>
+        </is>
+      </c>
+      <c r="H195" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="196">
+      <c r="A196" t="n">
+        <v>91</v>
+      </c>
+      <c r="B196" t="inlineStr">
+        <is>
+          <t>Stage X  Manual Welding of Backpieces at Bottom side of underframe</t>
+        </is>
+      </c>
+      <c r="C196" t="inlineStr">
+        <is>
+          <t>Underframe Welding Parts</t>
+        </is>
+      </c>
+      <c r="D196" t="inlineStr">
+        <is>
+          <t>1 11012.0.03.095.001</t>
+        </is>
+      </c>
+      <c r="E196" t="n">
+        <v>1</v>
+      </c>
+      <c r="F196" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="G196" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="H196" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="197">
+      <c r="A197" t="n">
+        <v>92</v>
+      </c>
+      <c r="B197" t="inlineStr">
+        <is>
+          <t>Stage XI Supporting members are welded at Topside of underframe</t>
+        </is>
+      </c>
+      <c r="C197" t="inlineStr">
+        <is>
+          <t>Supporting Members</t>
+        </is>
+      </c>
+      <c r="D197" t="inlineStr"/>
+      <c r="E197" t="n">
+        <v>1</v>
+      </c>
+      <c r="F197" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="G197" t="inlineStr">
+        <is>
+          <t>e</t>
+        </is>
+      </c>
+      <c r="H197" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="198">
+      <c r="A198" t="n">
+        <v>93</v>
+      </c>
+      <c r="B198" t="inlineStr">
+        <is>
+          <t>Stage XI Supporting members are welded at Topside of underframe</t>
+        </is>
+      </c>
+      <c r="C198" t="inlineStr">
+        <is>
+          <t>Supporting Members</t>
+        </is>
+      </c>
+      <c r="D198" t="inlineStr"/>
+      <c r="E198" t="n">
+        <v>1</v>
+      </c>
+      <c r="F198" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="G198" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+      <c r="H198" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="199">
+      <c r="A199" t="n">
+        <v>94</v>
+      </c>
+      <c r="B199" t="inlineStr">
+        <is>
+          <t>Stage XII  Final Inspection and attending of leftover work</t>
+        </is>
+      </c>
+      <c r="C199" t="inlineStr">
+        <is>
+          <t>Underframe frame work with corrugated sheet</t>
+        </is>
+      </c>
+      <c r="D199" t="inlineStr"/>
+      <c r="E199" t="n">
+        <v>1</v>
+      </c>
+      <c r="F199" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="G199" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="H199" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="200">
+      <c r="A200" t="n">
+        <v>95</v>
+      </c>
+      <c r="B200" t="inlineStr">
+        <is>
+          <t>Stage XII  Final Inspection and attending of leftover work</t>
+        </is>
+      </c>
+      <c r="C200" t="inlineStr">
+        <is>
+          <t>Underframe Welding Parts</t>
+        </is>
+      </c>
+      <c r="D200" t="inlineStr">
+        <is>
+          <t>1 11012.0.03.095.001</t>
+        </is>
+      </c>
+      <c r="E200" t="n">
+        <v>1</v>
+      </c>
+      <c r="F200" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="G200" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="H200" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="201">
+      <c r="A201" t="n">
+        <v>96</v>
+      </c>
+      <c r="B201" t="inlineStr">
+        <is>
+          <t>Stage XII  Final Inspection and attending of leftover work</t>
+        </is>
+      </c>
+      <c r="C201" t="inlineStr">
+        <is>
+          <t>Supporting Members</t>
+        </is>
+      </c>
+      <c r="D201" t="inlineStr"/>
+      <c r="E201" t="n">
+        <v>1</v>
+      </c>
+      <c r="F201" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="G201" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+      <c r="H201" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="202">
+      <c r="A202" t="n">
+        <v>97</v>
+      </c>
+      <c r="B202" t="inlineStr">
+        <is>
+          <t>Stage XII  Final Inspection and attending of leftover work</t>
+        </is>
+      </c>
+      <c r="C202" t="inlineStr">
+        <is>
+          <t>Underframe Complete</t>
+        </is>
+      </c>
+      <c r="D202" t="inlineStr">
+        <is>
+          <t>LE11105 alt h</t>
+        </is>
+      </c>
+      <c r="E202" t="n">
+        <v>1</v>
+      </c>
+      <c r="F202" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="G202" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="H202" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="203">
+      <c r="A203" t="n">
+        <v>98</v>
+      </c>
+      <c r="B203" t="inlineStr">
+        <is>
+          <t>Stage-I Robotic Shell AssemblyLine at 22.2.1 (JIG I &amp; II )</t>
+        </is>
+      </c>
+      <c r="C203" t="inlineStr">
+        <is>
+          <t>Side wall Left complete</t>
+        </is>
+      </c>
+      <c r="D203" t="inlineStr">
+        <is>
+          <t>LE14101 e</t>
+        </is>
+      </c>
+      <c r="E203" t="n">
+        <v>1</v>
+      </c>
+      <c r="F203" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="G203" t="n">
+        <v>4</v>
+      </c>
+      <c r="H203" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="204">
+      <c r="A204" t="n">
+        <v>99</v>
+      </c>
+      <c r="B204" t="inlineStr">
+        <is>
+          <t>Stage-I Robotic Shell AssemblyLine at 22.2.1 (JIG I &amp; II )</t>
+        </is>
+      </c>
+      <c r="C204" t="inlineStr">
+        <is>
+          <t>End wall Complete</t>
+        </is>
+      </c>
+      <c r="D204" t="inlineStr">
+        <is>
+          <t>1.10113.0.20.120.001</t>
+        </is>
+      </c>
+      <c r="E204" t="n">
+        <v>1</v>
+      </c>
+      <c r="F204" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="G204" t="n">
+        <v>5</v>
+      </c>
+      <c r="H204" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="205">
+      <c r="A205" t="n">
+        <v>100</v>
+      </c>
+      <c r="B205" t="inlineStr">
+        <is>
+          <t>Stage-I Robotic Shell AssemblyLine at 22.2.1 (JIG I &amp; II )</t>
+        </is>
+      </c>
+      <c r="C205" t="inlineStr">
+        <is>
+          <t>Roof Complete</t>
+        </is>
+      </c>
+      <c r="D205" t="inlineStr">
+        <is>
+          <t>LE16100 f</t>
+        </is>
+      </c>
+      <c r="E205" t="n">
+        <v>1</v>
+      </c>
+      <c r="F205" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="G205" t="n">
+        <v>6</v>
+      </c>
+      <c r="H205" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="206">
+      <c r="A206" t="n">
+        <v>101</v>
+      </c>
+      <c r="B206" t="inlineStr">
+        <is>
+          <t>Stage-I Robotic Shell AssemblyLine at 22.2.1 (JIG I &amp; II )</t>
+        </is>
+      </c>
+      <c r="C206" t="inlineStr">
+        <is>
+          <t>Underframe Complete</t>
+        </is>
+      </c>
+      <c r="D206" t="inlineStr">
+        <is>
+          <t>LE11105 alt h</t>
+        </is>
+      </c>
+      <c r="E206" t="n">
+        <v>1</v>
+      </c>
+      <c r="F206" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="G206" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="H206" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="207">
+      <c r="A207" t="n">
+        <v>102</v>
+      </c>
+      <c r="B207" t="inlineStr">
+        <is>
+          <t>Stage-I Robotic Shell AssemblyLine at 22.2.1 (JIG I &amp; II )</t>
+        </is>
+      </c>
+      <c r="C207" t="inlineStr">
+        <is>
+          <t>Shell Assembly</t>
+        </is>
+      </c>
+      <c r="D207" t="inlineStr"/>
+      <c r="E207" t="n">
+        <v>1</v>
+      </c>
+      <c r="F207" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="G207" t="n">
+        <v>1</v>
+      </c>
+      <c r="H207" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="208">
+      <c r="A208" t="n">
+        <v>103</v>
+      </c>
+      <c r="B208" t="inlineStr">
+        <is>
+          <t>Stage-II Final Repair &amp; Leakage testing</t>
+        </is>
+      </c>
+      <c r="C208" t="inlineStr">
+        <is>
+          <t>Shell Assembly</t>
+        </is>
+      </c>
+      <c r="D208" t="inlineStr"/>
+      <c r="E208" t="n">
+        <v>1</v>
+      </c>
+      <c r="F208" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="G208" t="n">
+        <v>1</v>
+      </c>
+      <c r="H208" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="209">
+      <c r="A209" t="n">
+        <v>104</v>
+      </c>
+      <c r="B209" t="inlineStr">
+        <is>
+          <t>Stage-II Final Repair &amp; Leakage testing</t>
+        </is>
+      </c>
+      <c r="C209" t="inlineStr">
+        <is>
+          <t>Coach</t>
+        </is>
+      </c>
+      <c r="D209" t="inlineStr"/>
+      <c r="E209" t="n">
+        <v>1</v>
+      </c>
+      <c r="F209" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="G209" t="n">
+        <v>1</v>
+      </c>
+      <c r="H209" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>